<commit_message>
Cleaned up the mess a bit
</commit_message>
<xml_diff>
--- a/orange_analysis/results.xlsx
+++ b/orange_analysis/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="113">
   <si>
     <t>Rule_expected</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>Galakrond's Awakening</t>
+  </si>
+  <si>
+    <t>Hearthstone_lemmas</t>
   </si>
 </sst>
 </file>
@@ -956,6 +959,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>% d'augmentation du vocabulaire</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -989,6 +1048,7 @@
         <c:crossAx val="-1832743344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -999,7 +1059,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3492,16 +3552,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>4535</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>193220</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>820963</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>162981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>816429</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>166309</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3522,16 +3582,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>4537</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>193223</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>820966</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>162984</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>816428</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>166309</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3816,11 +3876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC23"/>
+  <dimension ref="A1:CC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" zoomScale="84" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="84" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7575,6 +7635,11 @@
         <v>44.857113185993626</v>
       </c>
     </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Cleaned folders a bit
</commit_message>
<xml_diff>
--- a/orange_analysis/results.xlsx
+++ b/orange_analysis/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
   <si>
     <t>Rule_expected</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Galakrond's Awakening</t>
-  </si>
-  <si>
-    <t>Hearthstone_lemmas</t>
   </si>
 </sst>
 </file>
@@ -2304,7 +2301,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2382,7 +2379,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="-1832896688"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -3552,16 +3549,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>820963</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>162981</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4535</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>193219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>816429</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>166309</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>196547</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3582,16 +3579,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>820966</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>162984</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4537</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>193222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>816428</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>166309</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3876,11 +3873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC25"/>
+  <dimension ref="A1:CC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="84" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" zoomScale="84" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7635,11 +7632,6 @@
         <v>44.857113185993626</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>112</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>